<commit_message>
variable name table update
</commit_message>
<xml_diff>
--- a/SCAN/SCANHarvester/settings/variables.xlsx
+++ b/SCAN/SCANHarvester/settings/variables.xlsx
@@ -559,7 +559,7 @@
     <t xml:space="preserve">SMS_D_D10</t>
   </si>
   <si>
-    <t xml:space="preserve">Volumnometric water content</t>
+    <t xml:space="preserve">Volumetric water content </t>
   </si>
   <si>
     <t xml:space="preserve">SMS_D_D12</t>
@@ -2413,9 +2413,13 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -2437,8 +2441,8 @@
   </sheetPr>
   <dimension ref="A1:I713"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A343" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B33" activeCellId="0" sqref="B33"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A195" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B215" activeCellId="0" sqref="B215"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6287,7 +6291,7 @@
       <c r="A133" s="0" t="s">
         <v>178</v>
       </c>
-      <c r="B133" s="0" t="s">
+      <c r="B133" s="1" t="s">
         <v>179</v>
       </c>
       <c r="C133" s="0" t="s">
@@ -6316,7 +6320,7 @@
       <c r="A134" s="0" t="s">
         <v>180</v>
       </c>
-      <c r="B134" s="0" t="s">
+      <c r="B134" s="1" t="s">
         <v>179</v>
       </c>
       <c r="C134" s="0" t="s">
@@ -6345,7 +6349,7 @@
       <c r="A135" s="0" t="s">
         <v>181</v>
       </c>
-      <c r="B135" s="0" t="s">
+      <c r="B135" s="1" t="s">
         <v>179</v>
       </c>
       <c r="C135" s="0" t="s">
@@ -6374,7 +6378,7 @@
       <c r="A136" s="0" t="s">
         <v>182</v>
       </c>
-      <c r="B136" s="0" t="s">
+      <c r="B136" s="1" t="s">
         <v>179</v>
       </c>
       <c r="C136" s="0" t="s">
@@ -6403,7 +6407,7 @@
       <c r="A137" s="0" t="s">
         <v>183</v>
       </c>
-      <c r="B137" s="0" t="s">
+      <c r="B137" s="1" t="s">
         <v>179</v>
       </c>
       <c r="C137" s="0" t="s">
@@ -6432,7 +6436,7 @@
       <c r="A138" s="0" t="s">
         <v>184</v>
       </c>
-      <c r="B138" s="0" t="s">
+      <c r="B138" s="1" t="s">
         <v>179</v>
       </c>
       <c r="C138" s="0" t="s">
@@ -6461,7 +6465,7 @@
       <c r="A139" s="0" t="s">
         <v>185</v>
       </c>
-      <c r="B139" s="0" t="s">
+      <c r="B139" s="1" t="s">
         <v>179</v>
       </c>
       <c r="C139" s="0" t="s">
@@ -6490,7 +6494,7 @@
       <c r="A140" s="0" t="s">
         <v>186</v>
       </c>
-      <c r="B140" s="0" t="s">
+      <c r="B140" s="1" t="s">
         <v>179</v>
       </c>
       <c r="C140" s="0" t="s">
@@ -6519,7 +6523,7 @@
       <c r="A141" s="0" t="s">
         <v>187</v>
       </c>
-      <c r="B141" s="0" t="s">
+      <c r="B141" s="1" t="s">
         <v>179</v>
       </c>
       <c r="C141" s="0" t="s">
@@ -6548,7 +6552,7 @@
       <c r="A142" s="0" t="s">
         <v>188</v>
       </c>
-      <c r="B142" s="0" t="s">
+      <c r="B142" s="1" t="s">
         <v>179</v>
       </c>
       <c r="C142" s="0" t="s">
@@ -6577,7 +6581,7 @@
       <c r="A143" s="0" t="s">
         <v>189</v>
       </c>
-      <c r="B143" s="0" t="s">
+      <c r="B143" s="1" t="s">
         <v>179</v>
       </c>
       <c r="C143" s="0" t="s">
@@ -6606,7 +6610,7 @@
       <c r="A144" s="0" t="s">
         <v>190</v>
       </c>
-      <c r="B144" s="0" t="s">
+      <c r="B144" s="1" t="s">
         <v>179</v>
       </c>
       <c r="C144" s="0" t="s">
@@ -6635,7 +6639,7 @@
       <c r="A145" s="0" t="s">
         <v>191</v>
       </c>
-      <c r="B145" s="0" t="s">
+      <c r="B145" s="1" t="s">
         <v>179</v>
       </c>
       <c r="C145" s="0" t="s">
@@ -6664,7 +6668,7 @@
       <c r="A146" s="0" t="s">
         <v>192</v>
       </c>
-      <c r="B146" s="0" t="s">
+      <c r="B146" s="1" t="s">
         <v>179</v>
       </c>
       <c r="C146" s="0" t="s">
@@ -6693,7 +6697,7 @@
       <c r="A147" s="0" t="s">
         <v>193</v>
       </c>
-      <c r="B147" s="0" t="s">
+      <c r="B147" s="1" t="s">
         <v>179</v>
       </c>
       <c r="C147" s="0" t="s">
@@ -6722,7 +6726,7 @@
       <c r="A148" s="0" t="s">
         <v>194</v>
       </c>
-      <c r="B148" s="0" t="s">
+      <c r="B148" s="1" t="s">
         <v>179</v>
       </c>
       <c r="C148" s="0" t="s">
@@ -6751,7 +6755,7 @@
       <c r="A149" s="0" t="s">
         <v>195</v>
       </c>
-      <c r="B149" s="0" t="s">
+      <c r="B149" s="1" t="s">
         <v>179</v>
       </c>
       <c r="C149" s="0" t="s">
@@ -6780,7 +6784,7 @@
       <c r="A150" s="0" t="s">
         <v>196</v>
       </c>
-      <c r="B150" s="0" t="s">
+      <c r="B150" s="1" t="s">
         <v>179</v>
       </c>
       <c r="C150" s="0" t="s">
@@ -6809,7 +6813,7 @@
       <c r="A151" s="0" t="s">
         <v>197</v>
       </c>
-      <c r="B151" s="0" t="s">
+      <c r="B151" s="1" t="s">
         <v>179</v>
       </c>
       <c r="C151" s="0" t="s">
@@ -6838,7 +6842,7 @@
       <c r="A152" s="0" t="s">
         <v>198</v>
       </c>
-      <c r="B152" s="0" t="s">
+      <c r="B152" s="1" t="s">
         <v>179</v>
       </c>
       <c r="C152" s="0" t="s">
@@ -6867,7 +6871,7 @@
       <c r="A153" s="0" t="s">
         <v>199</v>
       </c>
-      <c r="B153" s="0" t="s">
+      <c r="B153" s="1" t="s">
         <v>179</v>
       </c>
       <c r="C153" s="0" t="s">
@@ -6896,7 +6900,7 @@
       <c r="A154" s="0" t="s">
         <v>200</v>
       </c>
-      <c r="B154" s="0" t="s">
+      <c r="B154" s="1" t="s">
         <v>179</v>
       </c>
       <c r="C154" s="0" t="s">
@@ -6925,7 +6929,7 @@
       <c r="A155" s="0" t="s">
         <v>201</v>
       </c>
-      <c r="B155" s="0" t="s">
+      <c r="B155" s="1" t="s">
         <v>179</v>
       </c>
       <c r="C155" s="0" t="s">
@@ -6954,7 +6958,7 @@
       <c r="A156" s="0" t="s">
         <v>202</v>
       </c>
-      <c r="B156" s="0" t="s">
+      <c r="B156" s="1" t="s">
         <v>179</v>
       </c>
       <c r="C156" s="0" t="s">
@@ -6983,7 +6987,7 @@
       <c r="A157" s="0" t="s">
         <v>203</v>
       </c>
-      <c r="B157" s="0" t="s">
+      <c r="B157" s="1" t="s">
         <v>179</v>
       </c>
       <c r="C157" s="0" t="s">
@@ -7012,7 +7016,7 @@
       <c r="A158" s="0" t="s">
         <v>204</v>
       </c>
-      <c r="B158" s="0" t="s">
+      <c r="B158" s="1" t="s">
         <v>179</v>
       </c>
       <c r="C158" s="0" t="s">
@@ -7041,7 +7045,7 @@
       <c r="A159" s="0" t="s">
         <v>205</v>
       </c>
-      <c r="B159" s="0" t="s">
+      <c r="B159" s="1" t="s">
         <v>179</v>
       </c>
       <c r="C159" s="0" t="s">
@@ -7070,7 +7074,7 @@
       <c r="A160" s="0" t="s">
         <v>206</v>
       </c>
-      <c r="B160" s="0" t="s">
+      <c r="B160" s="1" t="s">
         <v>179</v>
       </c>
       <c r="C160" s="0" t="s">
@@ -7099,7 +7103,7 @@
       <c r="A161" s="0" t="s">
         <v>207</v>
       </c>
-      <c r="B161" s="0" t="s">
+      <c r="B161" s="1" t="s">
         <v>179</v>
       </c>
       <c r="C161" s="0" t="s">
@@ -7128,7 +7132,7 @@
       <c r="A162" s="0" t="s">
         <v>208</v>
       </c>
-      <c r="B162" s="0" t="s">
+      <c r="B162" s="1" t="s">
         <v>179</v>
       </c>
       <c r="C162" s="0" t="s">
@@ -7157,7 +7161,7 @@
       <c r="A163" s="0" t="s">
         <v>209</v>
       </c>
-      <c r="B163" s="0" t="s">
+      <c r="B163" s="1" t="s">
         <v>179</v>
       </c>
       <c r="C163" s="0" t="s">
@@ -7186,7 +7190,7 @@
       <c r="A164" s="0" t="s">
         <v>210</v>
       </c>
-      <c r="B164" s="0" t="s">
+      <c r="B164" s="1" t="s">
         <v>179</v>
       </c>
       <c r="C164" s="0" t="s">
@@ -7215,7 +7219,7 @@
       <c r="A165" s="0" t="s">
         <v>211</v>
       </c>
-      <c r="B165" s="0" t="s">
+      <c r="B165" s="1" t="s">
         <v>179</v>
       </c>
       <c r="C165" s="0" t="s">
@@ -7244,7 +7248,7 @@
       <c r="A166" s="0" t="s">
         <v>212</v>
       </c>
-      <c r="B166" s="0" t="s">
+      <c r="B166" s="1" t="s">
         <v>179</v>
       </c>
       <c r="C166" s="0" t="s">
@@ -7273,7 +7277,7 @@
       <c r="A167" s="0" t="s">
         <v>213</v>
       </c>
-      <c r="B167" s="0" t="s">
+      <c r="B167" s="1" t="s">
         <v>179</v>
       </c>
       <c r="C167" s="0" t="s">
@@ -7302,7 +7306,7 @@
       <c r="A168" s="0" t="s">
         <v>214</v>
       </c>
-      <c r="B168" s="0" t="s">
+      <c r="B168" s="1" t="s">
         <v>179</v>
       </c>
       <c r="C168" s="0" t="s">
@@ -7331,7 +7335,7 @@
       <c r="A169" s="0" t="s">
         <v>215</v>
       </c>
-      <c r="B169" s="0" t="s">
+      <c r="B169" s="1" t="s">
         <v>179</v>
       </c>
       <c r="C169" s="0" t="s">
@@ -7360,7 +7364,7 @@
       <c r="A170" s="0" t="s">
         <v>216</v>
       </c>
-      <c r="B170" s="0" t="s">
+      <c r="B170" s="1" t="s">
         <v>179</v>
       </c>
       <c r="C170" s="0" t="s">
@@ -7389,7 +7393,7 @@
       <c r="A171" s="0" t="s">
         <v>217</v>
       </c>
-      <c r="B171" s="0" t="s">
+      <c r="B171" s="1" t="s">
         <v>179</v>
       </c>
       <c r="C171" s="0" t="s">
@@ -7418,7 +7422,7 @@
       <c r="A172" s="0" t="s">
         <v>218</v>
       </c>
-      <c r="B172" s="0" t="s">
+      <c r="B172" s="1" t="s">
         <v>179</v>
       </c>
       <c r="C172" s="0" t="s">
@@ -7447,7 +7451,7 @@
       <c r="A173" s="0" t="s">
         <v>219</v>
       </c>
-      <c r="B173" s="0" t="s">
+      <c r="B173" s="1" t="s">
         <v>179</v>
       </c>
       <c r="C173" s="0" t="s">
@@ -7476,7 +7480,7 @@
       <c r="A174" s="0" t="s">
         <v>220</v>
       </c>
-      <c r="B174" s="0" t="s">
+      <c r="B174" s="1" t="s">
         <v>179</v>
       </c>
       <c r="C174" s="0" t="s">
@@ -7505,7 +7509,7 @@
       <c r="A175" s="0" t="s">
         <v>221</v>
       </c>
-      <c r="B175" s="0" t="s">
+      <c r="B175" s="1" t="s">
         <v>179</v>
       </c>
       <c r="C175" s="0" t="s">
@@ -7534,7 +7538,7 @@
       <c r="A176" s="0" t="s">
         <v>222</v>
       </c>
-      <c r="B176" s="0" t="s">
+      <c r="B176" s="1" t="s">
         <v>179</v>
       </c>
       <c r="C176" s="0" t="s">
@@ -7563,7 +7567,7 @@
       <c r="A177" s="0" t="s">
         <v>223</v>
       </c>
-      <c r="B177" s="0" t="s">
+      <c r="B177" s="1" t="s">
         <v>179</v>
       </c>
       <c r="C177" s="0" t="s">
@@ -7592,7 +7596,7 @@
       <c r="A178" s="0" t="s">
         <v>224</v>
       </c>
-      <c r="B178" s="0" t="s">
+      <c r="B178" s="1" t="s">
         <v>179</v>
       </c>
       <c r="C178" s="0" t="s">
@@ -7621,7 +7625,7 @@
       <c r="A179" s="0" t="s">
         <v>225</v>
       </c>
-      <c r="B179" s="0" t="s">
+      <c r="B179" s="1" t="s">
         <v>179</v>
       </c>
       <c r="C179" s="0" t="s">
@@ -7650,7 +7654,7 @@
       <c r="A180" s="0" t="s">
         <v>226</v>
       </c>
-      <c r="B180" s="0" t="s">
+      <c r="B180" s="1" t="s">
         <v>179</v>
       </c>
       <c r="C180" s="0" t="s">
@@ -7679,7 +7683,7 @@
       <c r="A181" s="0" t="s">
         <v>227</v>
       </c>
-      <c r="B181" s="0" t="s">
+      <c r="B181" s="1" t="s">
         <v>179</v>
       </c>
       <c r="C181" s="0" t="s">
@@ -7708,7 +7712,7 @@
       <c r="A182" s="0" t="s">
         <v>228</v>
       </c>
-      <c r="B182" s="0" t="s">
+      <c r="B182" s="1" t="s">
         <v>179</v>
       </c>
       <c r="C182" s="0" t="s">
@@ -7737,7 +7741,7 @@
       <c r="A183" s="0" t="s">
         <v>229</v>
       </c>
-      <c r="B183" s="0" t="s">
+      <c r="B183" s="1" t="s">
         <v>179</v>
       </c>
       <c r="C183" s="0" t="s">
@@ -7766,7 +7770,7 @@
       <c r="A184" s="0" t="s">
         <v>230</v>
       </c>
-      <c r="B184" s="0" t="s">
+      <c r="B184" s="1" t="s">
         <v>179</v>
       </c>
       <c r="C184" s="0" t="s">
@@ -7795,7 +7799,7 @@
       <c r="A185" s="0" t="s">
         <v>231</v>
       </c>
-      <c r="B185" s="0" t="s">
+      <c r="B185" s="1" t="s">
         <v>179</v>
       </c>
       <c r="C185" s="0" t="s">
@@ -7824,7 +7828,7 @@
       <c r="A186" s="0" t="s">
         <v>232</v>
       </c>
-      <c r="B186" s="0" t="s">
+      <c r="B186" s="1" t="s">
         <v>179</v>
       </c>
       <c r="C186" s="0" t="s">
@@ -7853,7 +7857,7 @@
       <c r="A187" s="0" t="s">
         <v>233</v>
       </c>
-      <c r="B187" s="0" t="s">
+      <c r="B187" s="1" t="s">
         <v>179</v>
       </c>
       <c r="C187" s="0" t="s">
@@ -7882,7 +7886,7 @@
       <c r="A188" s="0" t="s">
         <v>234</v>
       </c>
-      <c r="B188" s="0" t="s">
+      <c r="B188" s="1" t="s">
         <v>179</v>
       </c>
       <c r="C188" s="0" t="s">
@@ -7911,7 +7915,7 @@
       <c r="A189" s="0" t="s">
         <v>235</v>
       </c>
-      <c r="B189" s="0" t="s">
+      <c r="B189" s="1" t="s">
         <v>179</v>
       </c>
       <c r="C189" s="0" t="s">
@@ -7940,7 +7944,7 @@
       <c r="A190" s="0" t="s">
         <v>236</v>
       </c>
-      <c r="B190" s="0" t="s">
+      <c r="B190" s="1" t="s">
         <v>179</v>
       </c>
       <c r="C190" s="0" t="s">
@@ -7969,7 +7973,7 @@
       <c r="A191" s="0" t="s">
         <v>237</v>
       </c>
-      <c r="B191" s="0" t="s">
+      <c r="B191" s="1" t="s">
         <v>179</v>
       </c>
       <c r="C191" s="0" t="s">
@@ -7998,7 +8002,7 @@
       <c r="A192" s="0" t="s">
         <v>238</v>
       </c>
-      <c r="B192" s="0" t="s">
+      <c r="B192" s="1" t="s">
         <v>179</v>
       </c>
       <c r="C192" s="0" t="s">
@@ -8027,7 +8031,7 @@
       <c r="A193" s="0" t="s">
         <v>239</v>
       </c>
-      <c r="B193" s="0" t="s">
+      <c r="B193" s="1" t="s">
         <v>179</v>
       </c>
       <c r="C193" s="0" t="s">
@@ -8056,7 +8060,7 @@
       <c r="A194" s="0" t="s">
         <v>240</v>
       </c>
-      <c r="B194" s="0" t="s">
+      <c r="B194" s="1" t="s">
         <v>179</v>
       </c>
       <c r="C194" s="0" t="s">
@@ -8085,7 +8089,7 @@
       <c r="A195" s="0" t="s">
         <v>241</v>
       </c>
-      <c r="B195" s="0" t="s">
+      <c r="B195" s="1" t="s">
         <v>179</v>
       </c>
       <c r="C195" s="0" t="s">
@@ -8114,7 +8118,7 @@
       <c r="A196" s="0" t="s">
         <v>242</v>
       </c>
-      <c r="B196" s="0" t="s">
+      <c r="B196" s="1" t="s">
         <v>179</v>
       </c>
       <c r="C196" s="0" t="s">
@@ -8143,7 +8147,7 @@
       <c r="A197" s="0" t="s">
         <v>243</v>
       </c>
-      <c r="B197" s="0" t="s">
+      <c r="B197" s="1" t="s">
         <v>179</v>
       </c>
       <c r="C197" s="0" t="s">
@@ -8172,7 +8176,7 @@
       <c r="A198" s="0" t="s">
         <v>244</v>
       </c>
-      <c r="B198" s="0" t="s">
+      <c r="B198" s="1" t="s">
         <v>179</v>
       </c>
       <c r="C198" s="0" t="s">
@@ -8201,7 +8205,7 @@
       <c r="A199" s="0" t="s">
         <v>245</v>
       </c>
-      <c r="B199" s="0" t="s">
+      <c r="B199" s="1" t="s">
         <v>179</v>
       </c>
       <c r="C199" s="0" t="s">
@@ -8230,7 +8234,7 @@
       <c r="A200" s="0" t="s">
         <v>246</v>
       </c>
-      <c r="B200" s="0" t="s">
+      <c r="B200" s="1" t="s">
         <v>179</v>
       </c>
       <c r="C200" s="0" t="s">
@@ -8259,7 +8263,7 @@
       <c r="A201" s="0" t="s">
         <v>247</v>
       </c>
-      <c r="B201" s="0" t="s">
+      <c r="B201" s="1" t="s">
         <v>179</v>
       </c>
       <c r="C201" s="0" t="s">
@@ -8288,7 +8292,7 @@
       <c r="A202" s="0" t="s">
         <v>248</v>
       </c>
-      <c r="B202" s="0" t="s">
+      <c r="B202" s="1" t="s">
         <v>179</v>
       </c>
       <c r="C202" s="0" t="s">
@@ -8317,7 +8321,7 @@
       <c r="A203" s="0" t="s">
         <v>249</v>
       </c>
-      <c r="B203" s="0" t="s">
+      <c r="B203" s="1" t="s">
         <v>179</v>
       </c>
       <c r="C203" s="0" t="s">
@@ -8346,7 +8350,7 @@
       <c r="A204" s="0" t="s">
         <v>250</v>
       </c>
-      <c r="B204" s="0" t="s">
+      <c r="B204" s="1" t="s">
         <v>179</v>
       </c>
       <c r="C204" s="0" t="s">
@@ -8375,7 +8379,7 @@
       <c r="A205" s="0" t="s">
         <v>251</v>
       </c>
-      <c r="B205" s="0" t="s">
+      <c r="B205" s="1" t="s">
         <v>179</v>
       </c>
       <c r="C205" s="0" t="s">
@@ -8404,7 +8408,7 @@
       <c r="A206" s="0" t="s">
         <v>252</v>
       </c>
-      <c r="B206" s="0" t="s">
+      <c r="B206" s="1" t="s">
         <v>179</v>
       </c>
       <c r="C206" s="0" t="s">
@@ -8433,7 +8437,7 @@
       <c r="A207" s="0" t="s">
         <v>253</v>
       </c>
-      <c r="B207" s="0" t="s">
+      <c r="B207" s="1" t="s">
         <v>179</v>
       </c>
       <c r="C207" s="0" t="s">
@@ -8462,7 +8466,7 @@
       <c r="A208" s="0" t="s">
         <v>254</v>
       </c>
-      <c r="B208" s="0" t="s">
+      <c r="B208" s="1" t="s">
         <v>179</v>
       </c>
       <c r="C208" s="0" t="s">
@@ -8491,7 +8495,7 @@
       <c r="A209" s="0" t="s">
         <v>255</v>
       </c>
-      <c r="B209" s="0" t="s">
+      <c r="B209" s="1" t="s">
         <v>179</v>
       </c>
       <c r="C209" s="0" t="s">
@@ -8520,7 +8524,7 @@
       <c r="A210" s="0" t="s">
         <v>256</v>
       </c>
-      <c r="B210" s="0" t="s">
+      <c r="B210" s="1" t="s">
         <v>179</v>
       </c>
       <c r="C210" s="0" t="s">
@@ -8549,7 +8553,7 @@
       <c r="A211" s="0" t="s">
         <v>257</v>
       </c>
-      <c r="B211" s="0" t="s">
+      <c r="B211" s="1" t="s">
         <v>179</v>
       </c>
       <c r="C211" s="0" t="s">
@@ -8578,7 +8582,7 @@
       <c r="A212" s="0" t="s">
         <v>258</v>
       </c>
-      <c r="B212" s="0" t="s">
+      <c r="B212" s="1" t="s">
         <v>179</v>
       </c>
       <c r="C212" s="0" t="s">

</xml_diff>

<commit_message>
update variable name for global radiation
</commit_message>
<xml_diff>
--- a/SCAN/SCANHarvester/settings/variables.xlsx
+++ b/SCAN/SCANHarvester/settings/variables.xlsx
@@ -820,7 +820,7 @@
     <t xml:space="preserve">SRADV_D</t>
   </si>
   <si>
-    <t xml:space="preserve">Radiation, incoming</t>
+    <t xml:space="preserve">Global Radiation</t>
   </si>
   <si>
     <t xml:space="preserve">SRADV_H</t>
@@ -2441,8 +2441,8 @@
   </sheetPr>
   <dimension ref="A1:I713"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A117" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B215" activeCellId="0" sqref="B215"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A360" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B224" activeCellId="0" sqref="B224"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
radiation variable name update
</commit_message>
<xml_diff>
--- a/SCAN/SCANHarvester/settings/variables.xlsx
+++ b/SCAN/SCANHarvester/settings/variables.xlsx
@@ -2441,8 +2441,8 @@
   </sheetPr>
   <dimension ref="A1:I713"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A360" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B224" activeCellId="0" sqref="B224"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
StandardDeviation correct name in controlled vocabulary
</commit_message>
<xml_diff>
--- a/SCAN/SCANHarvester/settings/variables.xlsx
+++ b/SCAN/SCANHarvester/settings/variables.xlsx
@@ -1690,7 +1690,7 @@
     <t xml:space="preserve">WDIRZ_D</t>
   </si>
   <si>
-    <t xml:space="preserve">Standard deviation</t>
+    <t xml:space="preserve">StandardDeviation</t>
   </si>
   <si>
     <t xml:space="preserve">WDIRZ_H</t>
@@ -2441,8 +2441,8 @@
   </sheetPr>
   <dimension ref="A1:I713"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A476" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E504" activeCellId="0" sqref="E504"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>